<commit_message>
Updated  InvalidTestData.xlsx for specific changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/InvalidTestData.xlsx
+++ b/src/test/resources/testdata/InvalidTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gojoko-my.sharepoint.com/personal/anil_kumar_gojokotech_com/Documents/Desktop/MCBAutomation/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="633" documentId="8_{BA21AB27-80F1-4ABF-91AB-1C4B23F0C3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F452044B-C33A-4B06-93D9-64B9EA18E86D}"/>
+  <xr:revisionPtr revIDLastSave="634" documentId="8_{BA21AB27-80F1-4ABF-91AB-1C4B23F0C3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A60CB86-C057-4666-BB7F-43ECC4849EB2}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A46C7419-73F4-47E5-82D4-5DD6C7D8EA23}"/>
   </bookViews>
@@ -4879,8 +4879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD5428A-76D9-401C-A3EA-36F3D393C743}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="V2" s="22">
         <f t="shared" ref="V2:V8" ca="1" si="0">(TODAY() - W2) + X2</f>
-        <v>29714</v>
+        <v>29715</v>
       </c>
       <c r="W2" s="22">
         <v>42818</v>
@@ -5132,7 +5132,7 @@
       </c>
       <c r="V3" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>29551</v>
+        <v>29552</v>
       </c>
       <c r="W3" s="22">
         <v>42818</v>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="V4" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>32401</v>
+        <v>32402</v>
       </c>
       <c r="W4" s="22">
         <v>42818</v>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="V5" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>34994</v>
+        <v>34995</v>
       </c>
       <c r="W5" s="22">
         <v>42818</v>
@@ -5366,7 +5366,7 @@
       </c>
       <c r="V6" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>31468</v>
+        <v>31469</v>
       </c>
       <c r="W6" s="22">
         <v>42818</v>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="V7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>32299</v>
+        <v>32300</v>
       </c>
       <c r="W7" s="22">
         <v>42818</v>
@@ -5522,7 +5522,7 @@
       </c>
       <c r="V8" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>31083</v>
+        <v>31084</v>
       </c>
       <c r="W8" s="22">
         <v>42818</v>
@@ -5677,7 +5677,7 @@
       </c>
       <c r="V10" s="22">
         <f ca="1">(TODAY() - W10) + X10</f>
-        <v>34823</v>
+        <v>34824</v>
       </c>
       <c r="W10" s="22">
         <v>42818</v>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="V11" s="22">
         <f ca="1">(TODAY() - W11) + X11</f>
-        <v>27322</v>
+        <v>27323</v>
       </c>
       <c r="W11" s="22">
         <v>42818</v>
@@ -6062,7 +6062,7 @@
         <v>1333</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>1377</v>
+        <v>1364</v>
       </c>
       <c r="M16" s="24" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
giignore file added and excel sheet updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/InvalidTestData.xlsx
+++ b/src/test/resources/testdata/InvalidTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gojoko-my.sharepoint.com/personal/anil_kumar_gojokotech_com/Documents/Desktop/MCBAutomation/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="634" documentId="8_{BA21AB27-80F1-4ABF-91AB-1C4B23F0C3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A60CB86-C057-4666-BB7F-43ECC4849EB2}"/>
+  <xr:revisionPtr revIDLastSave="665" documentId="8_{BA21AB27-80F1-4ABF-91AB-1C4B23F0C3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9DAB34A-37C9-4DD2-9203-8F215B0385E4}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A46C7419-73F4-47E5-82D4-5DD6C7D8EA23}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="1378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3575" uniqueCount="1396">
   <si>
     <t>Title</t>
   </si>
@@ -4183,6 +4183,60 @@
   </si>
   <si>
     <t>Less Than 3 Years Ago</t>
+  </si>
+  <si>
+    <t>Please select your loan purpose</t>
+  </si>
+  <si>
+    <t>Please select your title</t>
+  </si>
+  <si>
+    <t>Please confirm your first name</t>
+  </si>
+  <si>
+    <t>Please confirm your last name</t>
+  </si>
+  <si>
+    <t>Please enter a valid day</t>
+  </si>
+  <si>
+    <t>Please enter a valid month</t>
+  </si>
+  <si>
+    <t>Please enter a valid year</t>
+  </si>
+  <si>
+    <t>Please enter your email address</t>
+  </si>
+  <si>
+    <t>Please enter your UK mobile number</t>
+  </si>
+  <si>
+    <t>Please enter your postcode and click the button to find your address</t>
+  </si>
+  <si>
+    <t>Please select your address from the list</t>
+  </si>
+  <si>
+    <t>Please select when you moved in to this address</t>
+  </si>
+  <si>
+    <t>Please enter your income before tax, including any benefits you get</t>
+  </si>
+  <si>
+    <t>Please select</t>
+  </si>
+  <si>
+    <t>Please select what describes you best</t>
+  </si>
+  <si>
+    <t>Please enter your monthly rent/mortgage</t>
+  </si>
+  <si>
+    <t>Please enter your employer name</t>
+  </si>
+  <si>
+    <t>ExpectedValidationMes</t>
   </si>
 </sst>
 </file>
@@ -4366,7 +4420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4443,6 +4497,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4877,10 +4934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD5428A-76D9-401C-A3EA-36F3D393C743}">
-  <dimension ref="A1:Y22"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4904,14 +4961,15 @@
     <col min="19" max="19" width="18.7265625" style="24" customWidth="1"/>
     <col min="20" max="20" width="22.7265625" customWidth="1"/>
     <col min="21" max="21" width="12.26953125" style="24" customWidth="1"/>
-    <col min="22" max="22" width="12.08984375" style="24" customWidth="1"/>
-    <col min="23" max="23" width="14.81640625" style="24" customWidth="1"/>
-    <col min="24" max="24" width="11.7265625" style="24" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.81640625" style="24"/>
-    <col min="26" max="26" width="8.81640625" customWidth="1"/>
+    <col min="22" max="22" width="73.08984375" customWidth="1"/>
+    <col min="23" max="23" width="12.08984375" style="24" customWidth="1"/>
+    <col min="24" max="24" width="14.81640625" style="24" customWidth="1"/>
+    <col min="25" max="25" width="11.7265625" style="24" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.81640625" style="24"/>
+    <col min="27" max="27" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>1371</v>
       </c>
@@ -4975,20 +5033,23 @@
       <c r="U1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="5" t="s">
+        <v>1395</v>
+      </c>
+      <c r="W1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="X1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="24" t="s">
+      <c r="Y1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="24" t="s">
+      <c r="Z1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="b">
         <v>0</v>
       </c>
@@ -5052,21 +5113,24 @@
       <c r="U2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="22">
-        <f t="shared" ref="V2:V8" ca="1" si="0">(TODAY() - W2) + X2</f>
-        <v>29715</v>
+      <c r="V2" s="24" t="s">
+        <v>1378</v>
       </c>
       <c r="W2" s="22">
+        <f t="shared" ref="W2:W8" ca="1" si="0">(TODAY() - X2) + Y2</f>
+        <v>29716</v>
+      </c>
+      <c r="X2" s="22">
         <v>42818</v>
       </c>
-      <c r="X2" s="22">
+      <c r="Y2" s="22">
         <v>27065</v>
       </c>
-      <c r="Y2" s="24">
+      <c r="Z2" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -5130,21 +5194,24 @@
       <c r="U3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="22">
+      <c r="V3" s="24" t="s">
+        <v>1379</v>
+      </c>
+      <c r="W3" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>29552</v>
-      </c>
-      <c r="W3" s="22">
+        <v>29553</v>
+      </c>
+      <c r="X3" s="22">
         <v>42818</v>
       </c>
-      <c r="X3" s="22">
+      <c r="Y3" s="22">
         <v>26902</v>
       </c>
-      <c r="Y3" s="24">
+      <c r="Z3" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -5208,21 +5275,24 @@
       <c r="U4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V4" s="22">
+      <c r="V4" s="24" t="s">
+        <v>1380</v>
+      </c>
+      <c r="W4" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>32402</v>
-      </c>
-      <c r="W4" s="22">
+        <v>32403</v>
+      </c>
+      <c r="X4" s="22">
         <v>42818</v>
       </c>
-      <c r="X4" s="22">
+      <c r="Y4" s="22">
         <v>29752</v>
       </c>
-      <c r="Y4" s="24">
+      <c r="Z4" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -5286,21 +5356,24 @@
       <c r="U5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V5" s="22">
+      <c r="V5" s="24" t="s">
+        <v>1381</v>
+      </c>
+      <c r="W5" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>34995</v>
-      </c>
-      <c r="W5" s="22">
+        <v>34996</v>
+      </c>
+      <c r="X5" s="22">
         <v>42818</v>
       </c>
-      <c r="X5" s="22">
+      <c r="Y5" s="22">
         <v>32345</v>
       </c>
-      <c r="Y5" s="24">
+      <c r="Z5" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -5364,21 +5437,24 @@
       <c r="U6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V6" s="22">
+      <c r="V6" s="24" t="s">
+        <v>1382</v>
+      </c>
+      <c r="W6" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>31469</v>
-      </c>
-      <c r="W6" s="22">
+        <v>31470</v>
+      </c>
+      <c r="X6" s="22">
         <v>42818</v>
       </c>
-      <c r="X6" s="22">
+      <c r="Y6" s="22">
         <v>28819</v>
       </c>
-      <c r="Y6" s="24">
+      <c r="Z6" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -5442,21 +5518,24 @@
       <c r="U7" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V7" s="22">
+      <c r="V7" s="24" t="s">
+        <v>1383</v>
+      </c>
+      <c r="W7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>32300</v>
-      </c>
-      <c r="W7" s="22">
+        <v>32301</v>
+      </c>
+      <c r="X7" s="22">
         <v>42818</v>
       </c>
-      <c r="X7" s="22">
+      <c r="Y7" s="22">
         <v>29650</v>
       </c>
-      <c r="Y7" s="24">
+      <c r="Z7" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -5520,21 +5599,24 @@
       <c r="U8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V8" s="22">
+      <c r="V8" s="24" t="s">
+        <v>1384</v>
+      </c>
+      <c r="W8" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>31084</v>
-      </c>
-      <c r="W8" s="22">
+        <v>31085</v>
+      </c>
+      <c r="X8" s="22">
         <v>42818</v>
       </c>
-      <c r="X8" s="22">
+      <c r="Y8" s="22">
         <v>28434</v>
       </c>
-      <c r="Y8" s="24">
+      <c r="Z8" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -5598,20 +5680,23 @@
       <c r="U9" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V9" s="22">
+      <c r="V9" s="24" t="s">
+        <v>1385</v>
+      </c>
+      <c r="W9" s="22">
         <v>27</v>
       </c>
-      <c r="W9" s="22">
+      <c r="X9" s="22">
         <v>42818</v>
       </c>
-      <c r="X9" s="22">
+      <c r="Y9" s="22">
         <v>22100</v>
       </c>
-      <c r="Y9" s="24">
+      <c r="Z9" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -5675,21 +5760,24 @@
       <c r="U10" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V10" s="22">
-        <f ca="1">(TODAY() - W10) + X10</f>
-        <v>34824</v>
+      <c r="V10" s="24" t="s">
+        <v>1386</v>
       </c>
       <c r="W10" s="22">
+        <f ca="1">(TODAY() - X10) + Y10</f>
+        <v>34825</v>
+      </c>
+      <c r="X10" s="22">
         <v>42818</v>
       </c>
-      <c r="X10" s="22">
+      <c r="Y10" s="22">
         <v>32174</v>
       </c>
-      <c r="Y10" s="24">
+      <c r="Z10" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5753,21 +5841,24 @@
       <c r="U11" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V11" s="22">
-        <f ca="1">(TODAY() - W11) + X11</f>
-        <v>27323</v>
+      <c r="V11" s="40" t="s">
+        <v>1387</v>
       </c>
       <c r="W11" s="22">
+        <f ca="1">(TODAY() - X11) + Y11</f>
+        <v>27324</v>
+      </c>
+      <c r="X11" s="22">
         <v>42818</v>
       </c>
-      <c r="X11" s="22">
+      <c r="Y11" s="22">
         <v>24673</v>
       </c>
-      <c r="Y11" s="24">
+      <c r="Z11" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -5831,8 +5922,11 @@
       <c r="U12" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V12" s="24" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -5896,8 +5990,11 @@
       <c r="U13" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V13" s="24" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -5961,8 +6058,11 @@
       <c r="U14" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V14" s="24" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -6026,8 +6126,11 @@
       <c r="U15" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V15" s="24" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -6091,8 +6194,11 @@
       <c r="U16" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V16" s="24" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -6156,8 +6262,11 @@
       <c r="U17" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V17" s="24" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -6221,8 +6330,11 @@
       <c r="U18" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V18" s="24" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -6286,8 +6398,11 @@
       <c r="U19" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V19" s="24" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -6345,14 +6460,17 @@
       <c r="S20" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="T20" t="b">
+      <c r="T20" s="24" t="b">
         <v>0</v>
       </c>
       <c r="U20" s="24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V20" s="24" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -6416,8 +6534,11 @@
       <c r="U21" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V21" s="24" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -6480,6 +6601,9 @@
       </c>
       <c r="U22" s="24" t="b">
         <v>0</v>
+      </c>
+      <c r="V22" s="24" t="s">
+        <v>1394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>